<commit_message>
update model preprocessing with normalisation centered around zero
</commit_message>
<xml_diff>
--- a/trend_graph/CIFAR-100/momentum.xlsx
+++ b/trend_graph/CIFAR-100/momentum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xujingmao/Desktop/Pioneer Academics/Essay/Optimisation-of-Grid-Search-for-CNN-Hyperparameter-Tuning-in-Single-class-Image-Classification/trend_graph/CIFAR-100/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C3B43F7-A4B0-A945-A8B9-5B7BDC758A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2449EE49-9310-8F40-AC46-6FD7D29034D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="0" windowWidth="68800" windowHeight="28800" xr2:uid="{C0336E63-47A2-2142-96C7-F3DE0FA2FAB8}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{C0336E63-47A2-2142-96C7-F3DE0FA2FAB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2724,8 +2724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536A5753-564C-9547-B501-5038739FAC28}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="323" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="176" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>